<commit_message>
Remove : progressbar start
</commit_message>
<xml_diff>
--- a/app/AI Internal-Outputs/output.xlsx
+++ b/app/AI Internal-Outputs/output.xlsx
@@ -106,8 +106,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
-    <cellStyle hidden="0" name="6582644956526789746" xfId="1"/>
-    <cellStyle hidden="0" name="4674827761952396851" xfId="2"/>
+    <cellStyle hidden="0" name="7174450267964616321" xfId="1"/>
+    <cellStyle hidden="0" name="-4560894966670602496" xfId="2"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>

</xml_diff>